<commit_message>
adjusted moedeting and added .exe
</commit_message>
<xml_diff>
--- a/Gruppe/Mødetidting.xlsx
+++ b/Gruppe/Mødetidting.xlsx
@@ -457,12 +457,12 @@
   <dimension ref="A1:PR81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:K1048576"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" style="3"/>
     <col min="3" max="3" width="9.875" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="9" style="3"/>

</xml_diff>